<commit_message>
Added Knowledge - Data Link
</commit_message>
<xml_diff>
--- a/Phase 2 - Language Definition/language_definition.xlsx
+++ b/Phase 2 - Language Definition/language_definition.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="172">
   <si>
     <t>ID</t>
   </si>
@@ -247,13 +247,31 @@
     <t>KG-25-19</t>
   </si>
   <si>
-    <t>WheaterStation</t>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Severity of Anomaly</t>
+  </si>
+  <si>
+    <t>KG-25-20</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Name of city where there was the anomaly</t>
+  </si>
+  <si>
+    <t>KG-25-21</t>
+  </si>
+  <si>
+    <t>WeatherStation</t>
   </si>
   <si>
     <t>A physical location where instruments and sensors are installed to measure, record and monitor atmospheric parameters.</t>
   </si>
   <si>
-    <t>KG-25-20</t>
+    <t>KG-25-22</t>
   </si>
   <si>
     <t>Code</t>
@@ -262,7 +280,7 @@
     <t>The unique code of Weather Station.</t>
   </si>
   <si>
-    <t>KG-25-21</t>
+    <t>KG-25-23</t>
   </si>
   <si>
     <t>Name</t>
@@ -271,7 +289,7 @@
     <t>The name of Weather Station.</t>
   </si>
   <si>
-    <t>KG-25-22</t>
+    <t>KG-25-24</t>
   </si>
   <si>
     <t>Elevation</t>
@@ -293,7 +311,7 @@
     <t>The elevation of a location.</t>
   </si>
   <si>
-    <t>KG-25-23</t>
+    <t>KG-25-25</t>
   </si>
   <si>
     <t>Latitude</t>
@@ -315,7 +333,7 @@
     <t>The latitude of a location.</t>
   </si>
   <si>
-    <t>KG-25-24</t>
+    <t>KG-25-26</t>
   </si>
   <si>
     <t>Longitude</t>
@@ -337,7 +355,7 @@
     <t>The longitude of a location.</t>
   </si>
   <si>
-    <t>KG-25-25</t>
+    <t>KG-25-27</t>
   </si>
   <si>
     <t>StartDate</t>
@@ -349,7 +367,7 @@
     <t>The start date of the Weather Station data.</t>
   </si>
   <si>
-    <t>KG-25-26</t>
+    <t>KG-25-28</t>
   </si>
   <si>
     <t>EndDate</t>
@@ -371,7 +389,7 @@
     <t>The end date of the Weather Station data.</t>
   </si>
   <si>
-    <t>KG-25-27</t>
+    <t>KG-25-29</t>
   </si>
   <si>
     <t>MicroClimate</t>
@@ -380,7 +398,7 @@
     <t xml:space="preserve">A set of local atmospheric conditions that differ from those in the surrounding general area. </t>
   </si>
   <si>
-    <t>KG-25-28</t>
+    <t>KG-25-30</t>
   </si>
   <si>
     <t>TypeMicro</t>
@@ -389,7 +407,7 @@
     <t>Type of Microclimate.</t>
   </si>
   <si>
-    <t>KG-25-29</t>
+    <t>KG-25-31</t>
   </si>
   <si>
     <t>TemperatureRange</t>
@@ -401,7 +419,7 @@
     <t>The range of temperature of the day.</t>
   </si>
   <si>
-    <t>KG-25-30</t>
+    <t>KG-25-32</t>
   </si>
   <si>
     <t>HumidityRange</t>
@@ -410,7 +428,7 @@
     <t>The range of humidity of the day.</t>
   </si>
   <si>
-    <t>KG-25-31</t>
+    <t>KG-25-33</t>
   </si>
   <si>
     <t>WindPattern</t>
@@ -419,7 +437,7 @@
     <t>Patter of wind registered for that microclimate</t>
   </si>
   <si>
-    <t>KG-25-32</t>
+    <t>KG-25-34</t>
   </si>
   <si>
     <t>Region</t>
@@ -428,7 +446,7 @@
     <t>Code of Region.</t>
   </si>
   <si>
-    <t>KG-25-33</t>
+    <t>KG-25-35</t>
   </si>
   <si>
     <t>hasName - custom</t>
@@ -437,7 +455,7 @@
     <t>Name of Region.</t>
   </si>
   <si>
-    <t>KG-25-34</t>
+    <t>KG-25-36</t>
   </si>
   <si>
     <t>ClimateTrend</t>
@@ -446,7 +464,7 @@
     <t>The long-term pattern or direction of climate variables over a period of time.</t>
   </si>
   <si>
-    <t>KG-25-35</t>
+    <t>KG-25-37</t>
   </si>
   <si>
     <t>ParameterMeasured</t>
@@ -455,7 +473,7 @@
     <t>The specific weather or climate variables recorded to analyze the trend.</t>
   </si>
   <si>
-    <t>KG-25-36</t>
+    <t>KG-25-38</t>
   </si>
   <si>
     <t>TimeWindow</t>
@@ -464,7 +482,7 @@
     <t>The period over which the climate trend is observed or calculated.</t>
   </si>
   <si>
-    <t>KG-25-37</t>
+    <t>KG-25-39</t>
   </si>
   <si>
     <t>Variation</t>
@@ -473,7 +491,7 @@
     <t>The change or fluctuation in a weather parameter over time.</t>
   </si>
   <si>
-    <t>KG-25-38</t>
+    <t>KG-25-40</t>
   </si>
   <si>
     <t>Rate</t>
@@ -482,7 +500,7 @@
     <t>The speed at which a weather parameter changes within a given time window.</t>
   </si>
   <si>
-    <t>KG-25-39</t>
+    <t>KG-25-41</t>
   </si>
   <si>
     <t>Season</t>
@@ -492,7 +510,7 @@
 varying length of day and night. The fCustom season are: spring, summer, autumn and winter.</t>
   </si>
   <si>
-    <t>KG-25-40</t>
+    <t>KG-25-42</t>
   </si>
   <si>
     <t>Year</t>
@@ -501,7 +519,7 @@
     <t>Year of season.</t>
   </si>
   <si>
-    <t>KG-25-41</t>
+    <t>KG-25-43</t>
   </si>
   <si>
     <t>AverageTemperature</t>
@@ -510,7 +528,7 @@
     <t>Average temperature of season.</t>
   </si>
   <si>
-    <t>KG-25-42</t>
+    <t>KG-25-44</t>
   </si>
   <si>
     <t>AveragePrecipitation</t>
@@ -523,6 +541,54 @@
   </si>
   <si>
     <t>Data Source</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Generated</t>
+  </si>
+  <si>
+    <t>Anomaly type based on weather events per city.</t>
+  </si>
+  <si>
+    <t>Severity level calculated from anomaly intensity.</t>
+  </si>
+  <si>
+    <t>Shortname</t>
+  </si>
+  <si>
+    <t>Open Data Trentino</t>
+  </si>
+  <si>
+    <t>Local microclimate from temperature, humidity and wind data.</t>
+  </si>
+  <si>
+    <t>Microclimate classification from main weather ranges.</t>
+  </si>
+  <si>
+    <t>MeanTemperature</t>
+  </si>
+  <si>
+    <t>Temperature trend over the observation period.</t>
+  </si>
+  <si>
+    <t>VariationTime</t>
+  </si>
+  <si>
+    <t>Total temperature change from 1990 to 2025.</t>
+  </si>
+  <si>
+    <t>Annual temperature change rate.</t>
+  </si>
+  <si>
+    <t>Season assigned based on the date of measurement.</t>
+  </si>
+  <si>
+    <t>MeanPrecipitation</t>
   </si>
 </sst>
 </file>
@@ -604,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -626,14 +692,14 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -649,9 +715,6 @@
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1157,51 +1220,51 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22">
+    <row r="21" ht="16.5" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" ht="16.5" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1209,328 +1272,374 @@
       <c r="A25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="D28" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="D29" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="12" t="s">
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="C30" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="9" t="s">
+      <c r="A31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="9" t="s">
+      <c r="D33" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="9" t="s">
+      <c r="D34" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="9" t="s">
+    </row>
+    <row r="35">
+      <c r="A35" s="7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="C35" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="D35" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="9" t="s">
+      <c r="D37" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
+      <c r="D39" s="7" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C40" s="9" t="s">
+      <c r="A40" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="9" t="s">
+      <c r="D42" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C42" s="9" t="s">
+      <c r="D43" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C43" s="9" t="s">
+      <c r="D44" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44" s="9" t="s">
+      <c r="D45" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="9"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-    </row>
-    <row r="46" ht="25.5" customHeight="1">
-      <c r="A46" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="9" t="s">
+      <c r="D46" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="7"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+    </row>
+    <row r="48" ht="25.5" customHeight="1">
+      <c r="A48" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>147</v>
-      </c>
+      <c r="D51" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C3"/>
     <hyperlink r:id="rId2" ref="C20"/>
-    <hyperlink r:id="rId3" ref="C25"/>
-    <hyperlink r:id="rId4" ref="C26"/>
-    <hyperlink r:id="rId5" ref="C27"/>
-    <hyperlink r:id="rId6" ref="C29"/>
+    <hyperlink r:id="rId3" ref="C27"/>
+    <hyperlink r:id="rId4" ref="C28"/>
+    <hyperlink r:id="rId5" ref="C29"/>
+    <hyperlink r:id="rId6" ref="C31"/>
   </hyperlinks>
   <drawing r:id="rId7"/>
 </worksheet>
@@ -1546,9 +1655,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="27.38"/>
-    <col customWidth="1" min="3" max="3" width="41.38"/>
-    <col customWidth="1" min="4" max="4" width="39.88"/>
+    <col customWidth="1" min="2" max="2" width="23.63"/>
+    <col customWidth="1" min="3" max="3" width="26.88"/>
+    <col customWidth="1" min="4" max="4" width="44.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1559,10 +1668,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2">
@@ -1572,8 +1681,12 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
@@ -1582,8 +1695,12 @@
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
@@ -1592,8 +1709,12 @@
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
@@ -1602,8 +1723,12 @@
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
@@ -1612,8 +1737,12 @@
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
@@ -1622,7 +1751,12 @@
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
@@ -1631,8 +1765,12 @@
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
@@ -1641,8 +1779,12 @@
       <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
@@ -1651,7 +1793,12 @@
       <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="C10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
@@ -1660,18 +1807,26 @@
       <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
@@ -1680,8 +1835,12 @@
       <c r="B13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
@@ -1690,8 +1849,12 @@
       <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
@@ -1700,8 +1863,12 @@
       <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3"/>
@@ -1716,8 +1883,12 @@
       <c r="B17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
@@ -1726,8 +1897,12 @@
       <c r="B18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
@@ -1736,8 +1911,12 @@
       <c r="B19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
@@ -1746,275 +1925,406 @@
       <c r="B20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="9"/>
+      <c r="C26" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="A30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+      <c r="A31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
     </row>
     <row r="33">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+      <c r="C33" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+      <c r="C34" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="C35" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
+      <c r="A36" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
+      <c r="A37" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
+      <c r="A39" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
+      <c r="A40" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
     </row>
     <row r="42">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
+      <c r="C42" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="C43" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
+      <c r="C44" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="9"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
+      <c r="A45" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
+      <c r="A46" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
     </row>
     <row r="48">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="9"/>
+      <c r="C48" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
+      <c r="C49" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed images and files
</commit_message>
<xml_diff>
--- a/Phase 2 - Language Definition/language_definition.xlsx
+++ b/Phase 2 - Language Definition/language_definition.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Language Definition" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Knowledge - Data link" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Language Definition" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Knowledge - Data link" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -361,7 +361,7 @@
     <t>StartDate</t>
   </si>
   <si>
-    <t>Date - Schema.org</t>
+    <t>Date - W3.org</t>
   </si>
   <si>
     <t>The start date of the Weather Station data.</t>
@@ -382,7 +382,7 @@
         <color rgb="FF1155CC"/>
         <u/>
       </rPr>
-      <t>Schema.org</t>
+      <t>W3.org</t>
     </r>
   </si>
   <si>
@@ -395,6 +395,9 @@
     <t>MicroClimate</t>
   </si>
   <si>
+    <t xml:space="preserve">SweetOntology </t>
+  </si>
+  <si>
     <t xml:space="preserve">A set of local atmospheric conditions that differ from those in the surrounding general area. </t>
   </si>
   <si>
@@ -440,10 +443,7 @@
     <t>KG-25-34</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Code of Region.</t>
+    <t>City of Trentino Region</t>
   </si>
   <si>
     <t>KG-25-35</t>
@@ -452,7 +452,7 @@
     <t>hasName - custom</t>
   </si>
   <si>
-    <t>Name of Region.</t>
+    <t>Name of the city</t>
   </si>
   <si>
     <t>KG-25-36</t>
@@ -737,6 +737,10 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1380,66 +1384,66 @@
         <v>106</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38">
@@ -1450,10 +1454,10 @@
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>58</v>
@@ -2100,10 +2104,10 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>158</v>
@@ -2114,10 +2118,10 @@
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>165</v>
@@ -2128,10 +2132,10 @@
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>47</v>
@@ -2142,10 +2146,10 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>39</v>
@@ -2162,10 +2166,10 @@
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>161</v>

</xml_diff>